<commit_message>
update to new pyomo
parameter type in parameters declaration
intermediate variables as expressions
</commit_message>
<xml_diff>
--- a/Data/MainFile_ex.xlsx
+++ b/Data/MainFile_ex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cowi-my.sharepoint.com/personal/rapy_cowi_com/Documents/WHATIF/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapy\OneDrive - COWI\WHATIF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="13_ncr:1_{59A98145-E6ED-4466-95B7-E5F69A046B06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{80CF15EF-4F1A-4147-99DE-6F559813DCF9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A0BEEB-C3C5-43B2-9691-5CB732C073E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -3833,38 +3833,38 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.875" customWidth="1"/>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="4" width="11.25" customWidth="1"/>
-    <col min="5" max="5" width="10.625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="20.90625" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="11.375" customWidth="1"/>
-    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="18.75" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="56.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" ht="69" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>50</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>3</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>4</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="69">
         <v>6</v>
       </c>
@@ -4070,38 +4070,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="E20:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="60.75" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="2" width="60.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="52.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="C5" s="3" t="s">
         <v>68</v>
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>116</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>71</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>47</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="86" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" s="86" customFormat="1" ht="46" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>118</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>30</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>31</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" s="86" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A12" s="73" t="s">
         <v>132</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" ht="23" x14ac:dyDescent="0.25">
       <c r="A13" s="73" t="s">
         <v>84</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>62</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" ht="23" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
         <v>42</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" ht="23" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>59</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>69</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>100</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>81</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
         <v>60</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>101</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" s="86" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
         <v>131</v>
       </c>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="C22" s="79"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="77" t="s">
         <v>48</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>106</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A25" s="75" t="s">
         <v>43</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="46" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>74</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>76</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>77</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>73</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
         <v>61</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
         <v>67</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>63</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>44</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>45</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" s="86" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A35" s="98" t="s">
         <v>209</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>46</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
         <v>78</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>64</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>102</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="98" t="s">
         <v>186</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>104</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>103</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" s="86" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A43" s="75" t="s">
         <v>66</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" s="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
         <v>120</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" s="86" customFormat="1" ht="46" x14ac:dyDescent="0.25">
       <c r="A45" s="75" t="s">
         <v>130</v>
       </c>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="C45" s="81"/>
     </row>
-    <row r="46" spans="1:3" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" s="86" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A46" s="75" t="s">
         <v>115</v>
       </c>
@@ -4555,7 +4555,7 @@
       </c>
       <c r="C46" s="82"/>
     </row>
-    <row r="47" spans="1:3" ht="112.5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" ht="115" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
         <v>99</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="89.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="77" t="s">
         <v>108</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" s="86" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
         <v>111</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" s="86" customFormat="1" ht="23" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
         <v>128</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="86" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" s="86" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
         <v>129</v>
       </c>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="C51" s="79"/>
     </row>
-    <row r="52" spans="1:3" s="86" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" s="86" customFormat="1" ht="46" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
         <v>112</v>
       </c>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="C52" s="79"/>
     </row>
-    <row r="53" spans="1:3" s="86" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" s="86" customFormat="1" ht="46" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
         <v>189</v>
       </c>
@@ -4626,8 +4626,8 @@
       </c>
       <c r="C53" s="79"/>
     </row>
-    <row r="54" spans="1:3" ht="44.45" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" spans="1:3" ht="44.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4639,41 +4639,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AX23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.625" customWidth="1"/>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
-    <col min="3" max="4" width="11.875" style="86" customWidth="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
-    <col min="6" max="6" width="12.25" customWidth="1"/>
-    <col min="7" max="8" width="12.25" style="86" customWidth="1"/>
-    <col min="9" max="9" width="12.25" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
-    <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="9.5" customWidth="1"/>
-    <col min="13" max="13" width="8.25" customWidth="1"/>
-    <col min="14" max="14" width="11.125" customWidth="1"/>
-    <col min="15" max="15" width="11.75" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" style="86" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" customWidth="1"/>
+    <col min="7" max="8" width="12.26953125" style="86" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" customWidth="1"/>
+    <col min="14" max="14" width="11.08984375" customWidth="1"/>
+    <col min="15" max="15" width="11.7265625" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="10.75" customWidth="1"/>
-    <col min="18" max="18" width="11.5" customWidth="1"/>
-    <col min="19" max="19" width="11.125" customWidth="1"/>
-    <col min="20" max="20" width="11.25" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" customWidth="1"/>
+    <col min="18" max="18" width="11.453125" customWidth="1"/>
+    <col min="19" max="19" width="11.08984375" customWidth="1"/>
+    <col min="20" max="20" width="11.26953125" customWidth="1"/>
     <col min="21" max="21" width="10" customWidth="1"/>
-    <col min="22" max="22" width="11.375" customWidth="1"/>
-    <col min="23" max="23" width="12.875" customWidth="1"/>
-    <col min="24" max="24" width="14.25" customWidth="1"/>
-    <col min="25" max="25" width="11.75" customWidth="1"/>
-    <col min="26" max="26" width="10.625" customWidth="1"/>
-    <col min="27" max="27" width="12.75" customWidth="1"/>
-    <col min="28" max="28" width="12.5" customWidth="1"/>
+    <col min="22" max="22" width="11.36328125" customWidth="1"/>
+    <col min="23" max="23" width="12.90625" customWidth="1"/>
+    <col min="24" max="24" width="14.26953125" customWidth="1"/>
+    <col min="25" max="25" width="11.7265625" customWidth="1"/>
+    <col min="26" max="26" width="10.6328125" customWidth="1"/>
+    <col min="27" max="27" width="12.7265625" customWidth="1"/>
+    <col min="28" max="28" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -4682,7 +4682,7 @@
       <c r="D1" s="83"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
@@ -4718,7 +4718,7 @@
       <c r="AW2" s="4"/>
       <c r="AX2" s="4"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
@@ -4747,7 +4747,7 @@
       <c r="AW3" s="4"/>
       <c r="AX3" s="4"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>37</v>
       </c>
@@ -4795,7 +4795,7 @@
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="40"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -4841,7 +4841,7 @@
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>260</v>
       </c>
@@ -4887,7 +4887,7 @@
       <c r="AW6" s="4"/>
       <c r="AX6" s="4"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="120" t="s">
         <v>213</v>
       </c>
@@ -4935,7 +4935,7 @@
       <c r="AW7" s="4"/>
       <c r="AX7" s="4"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="41"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="15"/>
@@ -4967,7 +4967,7 @@
       <c r="AW8" s="4"/>
       <c r="AX8" s="4"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>261</v>
       </c>
@@ -5009,7 +5009,7 @@
       <c r="AW9" s="4"/>
       <c r="AX9" s="4"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="41"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -5055,7 +5055,7 @@
       <c r="AW10" s="4"/>
       <c r="AX10" s="4"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" s="41"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -5101,7 +5101,7 @@
       <c r="AW11" s="4"/>
       <c r="AX11" s="4"/>
     </row>
-    <row r="12" spans="1:50" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:50" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -5147,7 +5147,7 @@
       <c r="AW12" s="4"/>
       <c r="AX12" s="4"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -5193,7 +5193,7 @@
       <c r="AW13" s="4"/>
       <c r="AX13" s="4"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -5239,7 +5239,7 @@
       <c r="AW14" s="4"/>
       <c r="AX14" s="4"/>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
         <v>109</v>
       </c>
@@ -5287,7 +5287,7 @@
       <c r="AW15" s="4"/>
       <c r="AX15" s="4"/>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" s="71" t="s">
         <v>110</v>
       </c>
@@ -5334,7 +5334,7 @@
       <c r="AW16" s="4"/>
       <c r="AX16" s="4"/>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" s="71" t="s">
         <v>188</v>
       </c>
@@ -5382,7 +5382,7 @@
       <c r="AW17" s="4"/>
       <c r="AX17" s="4"/>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -5428,7 +5428,7 @@
       <c r="AW18" s="4"/>
       <c r="AX18" s="4"/>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
@@ -5457,7 +5457,7 @@
       <c r="AW19" s="4"/>
       <c r="AX19" s="4"/>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="Y20" s="4"/>
       <c r="Z20" s="47"/>
       <c r="AB20" s="4"/>
@@ -5484,7 +5484,7 @@
       <c r="AW20" s="4"/>
       <c r="AX20" s="4"/>
     </row>
-    <row r="22" spans="1:50" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
         <v>39</v>
       </c>
@@ -5530,7 +5530,7 @@
       <c r="AL22" s="87"/>
       <c r="AM22" s="87"/>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23" s="100" t="s">
         <v>275</v>
       </c>
@@ -5568,29 +5568,29 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="5" width="11.25" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="10.75" customWidth="1"/>
-    <col min="14" max="14" width="8.75" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="2" max="5" width="11.26953125" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="11" max="11" width="10.7265625" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>37</v>
       </c>
@@ -5605,7 +5605,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="55"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
@@ -5616,7 +5616,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="57"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -5629,7 +5629,7 @@
       <c r="H6" s="59"/>
       <c r="I6" s="60"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>269</v>
       </c>
@@ -5642,7 +5642,7 @@
       <c r="H7" s="61"/>
       <c r="I7" s="62"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>270</v>
       </c>
@@ -5655,7 +5655,7 @@
       <c r="H8" s="55"/>
       <c r="I8" s="56"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
         <v>263</v>
       </c>
@@ -5666,7 +5666,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="56"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
@@ -5677,7 +5677,7 @@
       <c r="H10" s="55"/>
       <c r="I10" s="56"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="55"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -5688,7 +5688,7 @@
       <c r="H11" s="61"/>
       <c r="I11" s="62"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="55"/>
       <c r="B12" s="55"/>
       <c r="C12" s="55"/>
@@ -5699,7 +5699,7 @@
       <c r="H12" s="63"/>
       <c r="I12" s="64"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="55"/>
       <c r="B13" s="55"/>
       <c r="C13" s="55"/>
@@ -5710,7 +5710,7 @@
       <c r="H13" s="63"/>
       <c r="I13" s="64"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="65"/>
       <c r="C14" s="65"/>
@@ -5721,7 +5721,7 @@
       <c r="H14" s="55"/>
       <c r="I14" s="64"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="55"/>
       <c r="C15" s="55"/>
@@ -5732,7 +5732,7 @@
       <c r="H15" s="55"/>
       <c r="I15" s="64"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="55"/>
       <c r="C16" s="55"/>
@@ -5743,7 +5743,7 @@
       <c r="H16" s="55"/>
       <c r="I16" s="64"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
       <c r="C17" s="55"/>
@@ -5754,7 +5754,7 @@
       <c r="H17" s="55"/>
       <c r="I17" s="56"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="53"/>
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
@@ -5765,10 +5765,10 @@
       <c r="H18" s="19"/>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>16</v>
       </c>
@@ -5782,7 +5782,7 @@
       <c r="G20" s="88"/>
       <c r="H20" s="88"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>0</v>
       </c>
@@ -5796,7 +5796,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>17</v>
       </c>
@@ -5810,7 +5810,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>113</v>
       </c>
@@ -5837,17 +5837,17 @@
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="14.125" customWidth="1"/>
-    <col min="11" max="11" width="10.375" customWidth="1"/>
-    <col min="13" max="13" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="83" t="s">
         <v>132</v>
       </c>
@@ -5872,7 +5872,7 @@
       <c r="T1" s="86"/>
       <c r="U1" s="86"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="84" t="s">
         <v>133</v>
       </c>
@@ -5897,7 +5897,7 @@
       <c r="T2" s="86"/>
       <c r="U2" s="86"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="84"/>
       <c r="B3" s="86"/>
       <c r="C3" s="86"/>
@@ -5920,7 +5920,7 @@
       <c r="T3" s="86"/>
       <c r="U3" s="86"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>37</v>
       </c>
@@ -5947,7 +5947,7 @@
       <c r="T4" s="86"/>
       <c r="U4" s="86"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="86" t="s">
         <v>265</v>
       </c>
@@ -5972,7 +5972,7 @@
       <c r="T5" s="86"/>
       <c r="U5" s="86"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="86" t="s">
         <v>266</v>
       </c>
@@ -5983,7 +5983,7 @@
       <c r="F6" s="95"/>
       <c r="AB6" s="86"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>271</v>
       </c>
@@ -5994,7 +5994,7 @@
       <c r="F7" s="95"/>
       <c r="AB7" s="86"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -6005,7 +6005,7 @@
       <c r="F8" s="95"/>
       <c r="AB8" s="86"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>273</v>
       </c>
@@ -6016,7 +6016,7 @@
       <c r="F9" s="4"/>
       <c r="AB9" s="86"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
       <c r="D10" s="56"/>
@@ -6038,7 +6038,7 @@
       <c r="T10" s="86"/>
       <c r="U10" s="86"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B11" s="86"/>
       <c r="C11" s="86"/>
       <c r="D11" s="51"/>
@@ -6060,7 +6060,7 @@
       <c r="T11" s="86"/>
       <c r="U11" s="86"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="D12" s="56"/>
       <c r="E12" s="55"/>
@@ -6081,7 +6081,7 @@
       <c r="T12" s="86"/>
       <c r="U12" s="86"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="129" t="s">
         <v>274</v>
       </c>
@@ -6105,7 +6105,7 @@
       <c r="T13" s="86"/>
       <c r="U13" s="86"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="127" t="s">
         <v>267</v>
       </c>
@@ -6128,7 +6128,7 @@
       <c r="T14" s="86"/>
       <c r="U14" s="86"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
         <v>134</v>
       </c>
@@ -6153,7 +6153,7 @@
       <c r="T15" s="86"/>
       <c r="U15" s="86"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>135</v>
       </c>
@@ -6178,7 +6178,7 @@
       <c r="T16" s="86"/>
       <c r="U16" s="86"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
       <c r="C17" s="55"/>
@@ -6201,7 +6201,7 @@
       <c r="T17" s="86"/>
       <c r="U17" s="86"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="53"/>
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
@@ -6224,7 +6224,7 @@
       <c r="T18" s="86"/>
       <c r="U18" s="86"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="84"/>
       <c r="B19" s="86"/>
       <c r="C19" s="86"/>
@@ -6247,7 +6247,7 @@
       <c r="T19" s="86"/>
       <c r="U19" s="86"/>
     </row>
-    <row r="20" spans="1:21" ht="112.5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" ht="126.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>16</v>
       </c>
@@ -6304,7 +6304,7 @@
       </c>
       <c r="U20" s="86"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="85" t="s">
         <v>0</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>158</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>179</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -6536,12 +6536,12 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="83" t="s">
         <v>121</v>
       </c>
@@ -6571,19 +6571,19 @@
       <c r="AB1" s="5"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="84" t="s">
         <v>264</v>
       </c>
       <c r="B2" s="86"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="90" t="s">
         <v>122</v>
       </c>
       <c r="B3" s="86"/>
     </row>
-    <row r="4" spans="1:29" ht="46.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
@@ -6593,13 +6593,13 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="85" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="86"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>124</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="91">
         <v>1</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="91">
         <v>2</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="91">
         <v>3</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="91">
         <v>4</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="91">
         <v>5</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="91">
         <v>6</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="91">
         <v>7</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="91">
         <v>8</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="91">
         <v>9</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="91">
         <v>10</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="91">
         <v>11</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="91">
         <v>12</v>
       </c>
@@ -6703,76 +6703,76 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
   </sheetData>
@@ -6788,14 +6788,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="101" t="s">
         <v>203</v>
       </c>
@@ -6814,7 +6814,7 @@
       <c r="N1" s="69"/>
       <c r="O1" s="69"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>82</v>
       </c>
@@ -6833,7 +6833,7 @@
       <c r="N2" s="69"/>
       <c r="O2" s="69"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="103"/>
       <c r="B3" s="69"/>
       <c r="C3" s="69"/>
@@ -6850,7 +6850,7 @@
       <c r="N3" s="69"/>
       <c r="O3" s="69"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="104" t="s">
         <v>37</v>
       </c>
@@ -6869,7 +6869,7 @@
       <c r="N4" s="105"/>
       <c r="O4" s="106"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="107"/>
       <c r="B5" s="108"/>
       <c r="C5" s="108"/>
@@ -6886,7 +6886,7 @@
       <c r="N5" s="108"/>
       <c r="O5" s="109"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="126" t="s">
         <v>262</v>
       </c>
@@ -6905,7 +6905,7 @@
       <c r="N6" s="108"/>
       <c r="O6" s="109"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="110"/>
       <c r="B7" s="108"/>
       <c r="C7" s="108"/>
@@ -6922,7 +6922,7 @@
       <c r="N7" s="108"/>
       <c r="O7" s="109"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="110"/>
       <c r="B8" s="69"/>
       <c r="C8" s="69"/>
@@ -6939,7 +6939,7 @@
       <c r="N8" s="69"/>
       <c r="O8" s="109"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="110"/>
       <c r="B9" s="108"/>
       <c r="C9" s="108"/>
@@ -6956,7 +6956,7 @@
       <c r="N9" s="69"/>
       <c r="O9" s="109"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="110"/>
       <c r="B10" s="108"/>
       <c r="C10" s="108"/>
@@ -6973,7 +6973,7 @@
       <c r="N10" s="108"/>
       <c r="O10" s="109"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="110"/>
       <c r="B11" s="86"/>
       <c r="C11" s="108"/>
@@ -6990,7 +6990,7 @@
       <c r="N11" s="108"/>
       <c r="O11" s="109"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
       <c r="B12" s="86"/>
       <c r="C12" s="108"/>
@@ -7007,7 +7007,7 @@
       <c r="N12" s="108"/>
       <c r="O12" s="109"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="110"/>
       <c r="B13" s="69"/>
       <c r="C13" s="108"/>
@@ -7024,7 +7024,7 @@
       <c r="N13" s="108"/>
       <c r="O13" s="109"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="110"/>
       <c r="B14" s="108"/>
       <c r="C14" s="108"/>
@@ -7041,7 +7041,7 @@
       <c r="N14" s="108"/>
       <c r="O14" s="109"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="110"/>
       <c r="B15" s="108"/>
       <c r="C15" s="108"/>
@@ -7058,7 +7058,7 @@
       <c r="N15" s="108"/>
       <c r="O15" s="109"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="110"/>
       <c r="B16" s="108"/>
       <c r="C16" s="108"/>
@@ -7075,7 +7075,7 @@
       <c r="N16" s="108"/>
       <c r="O16" s="109"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="110"/>
       <c r="B17" s="108"/>
       <c r="C17" s="108"/>
@@ -7092,7 +7092,7 @@
       <c r="N17" s="108"/>
       <c r="O17" s="109"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="111"/>
       <c r="B18" s="112"/>
       <c r="C18" s="112"/>
@@ -7109,7 +7109,7 @@
       <c r="N18" s="112"/>
       <c r="O18" s="113"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="114"/>
       <c r="B19" s="69"/>
       <c r="C19" s="69"/>
@@ -7126,7 +7126,7 @@
       <c r="N19" s="69"/>
       <c r="O19" s="69"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="69"/>
       <c r="B20" s="69"/>
       <c r="C20" s="69"/>
@@ -7143,7 +7143,7 @@
       <c r="N20" s="69"/>
       <c r="O20" s="69"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="69"/>
       <c r="C21" s="69"/>
@@ -7160,7 +7160,7 @@
       <c r="N21" s="69"/>
       <c r="O21" s="69"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
         <v>204</v>
       </c>
@@ -7185,7 +7185,7 @@
       <c r="N22" s="69"/>
       <c r="O22" s="69"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="87" t="s">
         <v>211</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="87"/>
       <c r="B24" s="86">
         <v>2</v>
@@ -7211,7 +7211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="87"/>
       <c r="B25" s="86">
         <v>3</v>
@@ -7223,7 +7223,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="87" t="s">
         <v>212</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="87"/>
       <c r="B27" s="86">
         <v>2</v>
@@ -7249,7 +7249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="87"/>
       <c r="B28" s="86">
         <v>3</v>
@@ -7261,7 +7261,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>194</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="86">
         <v>2</v>
@@ -7287,7 +7287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="86">
         <v>3</v>
@@ -7299,7 +7299,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="87" t="s">
         <v>196</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="87"/>
       <c r="B33" s="86">
         <v>2</v>
@@ -7325,7 +7325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="87"/>
       <c r="B34" s="86">
         <v>3</v>
@@ -7337,7 +7337,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>193</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="86">
         <v>2</v>
@@ -7363,7 +7363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="86" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="86">
         <v>3</v>
@@ -7375,7 +7375,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>195</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="86">
         <v>2</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="86">
         <v>3</v>
       </c>
@@ -7411,13 +7411,13 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="86"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="86"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="86"/>
     </row>
   </sheetData>
@@ -7433,31 +7433,31 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
-    <col min="2" max="3" width="13.875" customWidth="1"/>
-    <col min="4" max="4" width="11.25" customWidth="1"/>
-    <col min="5" max="5" width="10.625" customWidth="1"/>
-    <col min="6" max="6" width="10.125" customWidth="1"/>
-    <col min="7" max="7" width="12.875" customWidth="1"/>
-    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
+    <col min="2" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>37</v>
       </c>
@@ -7472,7 +7472,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="55"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
@@ -7483,7 +7483,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="57"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="92" t="s">
         <v>126</v>
       </c>
@@ -7496,7 +7496,7 @@
       <c r="H6" s="59"/>
       <c r="I6" s="60"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="58"/>
@@ -7507,7 +7507,7 @@
       <c r="I7" s="69"/>
       <c r="J7" s="69"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="58"/>
@@ -7518,7 +7518,7 @@
       <c r="I8" s="69"/>
       <c r="J8" s="69"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="51"/>
       <c r="E9" s="69"/>
       <c r="F9" s="69"/>
@@ -7527,7 +7527,7 @@
       <c r="I9" s="69"/>
       <c r="J9" s="69"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="71" t="s">
         <v>94</v>
       </c>
@@ -7541,7 +7541,7 @@
       <c r="I10" s="69"/>
       <c r="J10" s="69"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="68" t="s">
         <v>98</v>
       </c>
@@ -7555,7 +7555,7 @@
       <c r="I11" s="69"/>
       <c r="J11" s="69"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
         <v>96</v>
       </c>
@@ -7569,7 +7569,7 @@
       <c r="I12" s="69"/>
       <c r="J12" s="69"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="72" t="s">
         <v>97</v>
       </c>
@@ -7583,7 +7583,7 @@
       <c r="I13" s="69"/>
       <c r="J13" s="69"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="65"/>
       <c r="C14" s="65"/>
@@ -7595,7 +7595,7 @@
       <c r="I14" s="69"/>
       <c r="J14" s="69"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="55"/>
       <c r="C15" s="55"/>
@@ -7607,7 +7607,7 @@
       <c r="I15" s="69"/>
       <c r="J15" s="69"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="55"/>
       <c r="C16" s="55"/>
@@ -7619,7 +7619,7 @@
       <c r="I16" s="69"/>
       <c r="J16" s="69"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
       <c r="C17" s="55"/>
@@ -7630,7 +7630,7 @@
       <c r="H17" s="55"/>
       <c r="I17" s="56"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="53"/>
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
@@ -7641,7 +7641,7 @@
       <c r="H18" s="19"/>
       <c r="I18" s="20"/>
     </row>
-    <row r="20" spans="1:9" ht="56.25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="57.5" x14ac:dyDescent="0.25">
       <c r="A20" s="86"/>
       <c r="B20" s="25" t="s">
         <v>89</v>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="G20" s="25"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="86"/>
       <c r="B21" s="86" t="s">
         <v>13</v>
@@ -7671,7 +7671,7 @@
       <c r="F21" s="86"/>
       <c r="G21" s="86"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>95</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="s">
         <v>114</v>
       </c>
@@ -7717,21 +7717,21 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="44"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="44"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="44"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="44"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="44"/>
       <c r="H42" s="4"/>
     </row>

</xml_diff>